<commit_message>
Cote d'Ivoire spelling updated
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="115">
   <si>
     <t>Name</t>
   </si>
@@ -115,139 +115,142 @@
     <t>Endeva</t>
   </si>
   <si>
+    <t>Afghanistan, Armenia, Azerbaijan, Bahrain, Bangladesh, Bhutan, Brunei, Cambodia, China, Cyprus, Georgia, India, Indonesia, Iran, Iraq, Israel, Japan, Jordan, Kazakhstan, Kuwait, Kyrgyzstan, Laos, Lebanon, Malaysia, Maldives, Mongolia, Myanmar, Nepal, Oman, Pakistan, Palestine, Philippines, Qatar, Russia, Saudi Arabia, Singapore, Dem. Rep. Korea, Sri Lanka, Syria, Taiwan, Tajikistan, Thailand, Timor-Leste, Turkey, Turkmenistan, United Arab Emirates, Uzbekistan, Vietnam, Yemen, Algeria, Angola, Benin, Botswana, Burkina Faso, Burundi, Cabo Verde, Cameroon, Central African Rep., Chad, Comoros, Dem. Rep. Congo, Congo, Cote d'Ivoire, Djibouti, Egypt, Eq. Guinea, Eritrea, Swaziland, Ethiopia, Gabon, Gambia, Ghana, Guinea, Guinea-Bissau, Kenya, Lesotho, Liberia, Libya, Madagascar, Malawi, Mali, Mauritania, Mauritius, Morocco, Mozambique, Namibia, Niger, Nigeria, Rwanda, Sao Tome and Principe, Senegal, Seychelles, Sierra Leone, Somalia, South Africa, S. Sudan, Sudan, Tanzania, Togo, Tunisia, Uganda, Zambia, Zimbabwe, Algeria, Bahrain, Egypt, Iran, Iraq, Israel, Brazil, Bolivia, Chile, Colombia, Costa Rica, Cuba, Dominican Rep., Ecuador, El Salvador, Guinea, Guatemala, Honduras, Martinique, Mexico, Nicaragua, Panama, Paraguay, Peru, Puerto Rico, Uruguay, Venezuela, Albania, Armenia, Azerbaijan, Belarus, Georgia, Kazakhstan, Kosovo, Kyrgyzstan, Macedonia, Moldova, Montenegro, Russia, Serbia, Tajikistan, Turkmenistan, Ukraine, Uzbekistan, Argentina</t>
+  </si>
+  <si>
+    <t>Entrepreneurship School (Social Entrepreneurship)</t>
+  </si>
+  <si>
+    <t>online</t>
+  </si>
+  <si>
+    <t>Enviu</t>
+  </si>
+  <si>
+    <t>Netherlands, Nairobi, Kenya, India, USA</t>
+  </si>
+  <si>
+    <t>Euforia</t>
+  </si>
+  <si>
+    <t>Switzerland, Rwanda, Egypt, Greece, Turkey, Austria, Netherlands, P. of Liechtenstein, France, Germany, Portugal, Colombia, Peru, Bolivia</t>
+  </si>
+  <si>
+    <t>European Social Innovation Competition</t>
+  </si>
+  <si>
+    <t>Iceland, Norway, Albania, Bosnia and Herz., Macedonia, Montenegro, Serbia, Turkey, Israel, Moldova, Switzerland, Faroe Islands, Ukraine, Tunisia, Georgia, Armenia</t>
+  </si>
+  <si>
+    <t>EY - Entrepreneur of the Year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Canada, Indonesia, Philippines </t>
+  </si>
+  <si>
+    <t>Facebook Social Entrepreneurship Award</t>
+  </si>
+  <si>
+    <t>Fledge</t>
+  </si>
+  <si>
+    <t>Peru, Spain, Italy, Canada, USA</t>
+  </si>
+  <si>
+    <t>Fossil Foundation</t>
+  </si>
+  <si>
+    <t>Canada, USA, Ecuador, Zambia, Kenya, Nigeria, Italy, Switzerland, UK, Poland, India, Cambodia, Laos, China, Hong Kong, Taiwan</t>
+  </si>
+  <si>
+    <t>Global Social Entrepreneurship Network</t>
+  </si>
+  <si>
+    <t>Canada, USA, Europe, Chile, South Africa, Tanzania, Congo, Chad, Morocco, Israel, Cyprus, China, Dem. Rep. Korea, Thailand, Malaysia, Indonesia, Australia, New Zealand, Taiwan</t>
+  </si>
+  <si>
+    <t>Costs</t>
+  </si>
+  <si>
+    <t>Online Courses (1= nur online, 2= beides)</t>
+  </si>
+  <si>
+    <t>Europe</t>
+  </si>
+  <si>
+    <t>Global Social Venture Competition</t>
+  </si>
+  <si>
+    <t>Global Center for Social Entrepreneurship Networks (GCSEN)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Halcyon </t>
+  </si>
+  <si>
+    <t>USA, Saudi Arabia, Dem. Rep. Korea</t>
+  </si>
+  <si>
+    <t>HKCSS Impact Incubator</t>
+  </si>
+  <si>
+    <t>Hult Prize</t>
+  </si>
+  <si>
+    <t>Impact Engine</t>
+  </si>
+  <si>
+    <t>Canada, USA</t>
+  </si>
+  <si>
+    <t>Makesense</t>
+  </si>
+  <si>
+    <t>USA, Canada, Mexico, Dominican Rep., Nicaragua, Guatemala, Trinidad and Tobago, Colombia, Argentina, Paraguay, Brazil, Europe, Morocco, Tunisia, South Africa, Australia, Lebanon, Mali, Burkina Faso, Cote d'Ivoire, Senegal, Togo, Uganda, Kenya, Egypt, Turkey, Armenia, Teheran, Nepal, India, China, Myanmar, Cambodia, Vietnam, Malaysia, Singapore, Indonesia, Philippines, Dem. Rep. Korea, Japan, New Zealand</t>
+  </si>
+  <si>
+    <t>MassChallenge</t>
+  </si>
+  <si>
+    <t>USA, Israel, Mexico, Switzerland, UK</t>
+  </si>
+  <si>
+    <t>Middlesex University London (Social Enterprise: Turning Ideas into Action)</t>
+  </si>
+  <si>
+    <t>Miller Center for Social Entrepreneurship - Global Social Benefit Institute</t>
+  </si>
+  <si>
+    <t>Ogunte</t>
+  </si>
+  <si>
+    <t>Orange Social Venture Prize</t>
+  </si>
+  <si>
+    <t>Morocco, Tunisia, Egypt, Senegal, Botswana, Liberia, cote d'ivoire, Cameroon, Mali, Guinea , Guinea-Bissau, Madagascar, Niger, Central African Rep., Dem. Rep. Congo, Jordan, Burkina Faso</t>
+  </si>
+  <si>
+    <t>Acumen</t>
+  </si>
+  <si>
+    <t>Schwab Foundation for Social Entrepreneurship</t>
+  </si>
+  <si>
+    <t>Seakademie</t>
+  </si>
+  <si>
+    <t>Mexico, South Africa, China, Germany</t>
+  </si>
+  <si>
+    <t>SEED Initiative</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Colombia, India, Tanzania, Thailand, Uganda </t>
+  </si>
+  <si>
+    <t>Seedstars</t>
+  </si>
+  <si>
     <t>Afghanistan, Armenia, Azerbaijan, Bahrain, Bangladesh, Bhutan, Brunei, Cambodia, China, Cyprus, Georgia, India, Indonesia, Iran, Iraq, Israel, Japan, Jordan, Kazakhstan, Kuwait, Kyrgyzstan, Laos, Lebanon, Malaysia, Maldives, Mongolia, Myanmar, Nepal, Oman, Pakistan, Palestine, Philippines, Qatar, Russia, Saudi Arabia, Singapore, Dem. Rep. Korea, Sri Lanka, Syria, Taiwan, Tajikistan, Thailand, Timor-Leste, Turkey, Turkmenistan, United Arab Emirates, Uzbekistan, Vietnam, Yemen, Algeria, Angola, Benin, Botswana, Burkina Faso, Burundi, Cabo Verde, Cameroon, Central African Rep., Chad, Comoros, Dem. Rep. Congo, Congo, Cote d’Ivoire, Djibouti, Egypt, Eq. Guinea, Eritrea, Swaziland, Ethiopia, Gabon, Gambia, Ghana, Guinea, Guinea-Bissau, Kenya, Lesotho, Liberia, Libya, Madagascar, Malawi, Mali, Mauritania, Mauritius, Morocco, Mozambique, Namibia, Niger, Nigeria, Rwanda, Sao Tome and Principe, Senegal, Seychelles, Sierra Leone, Somalia, South Africa, S. Sudan, Sudan, Tanzania, Togo, Tunisia, Uganda, Zambia, Zimbabwe, Algeria, Bahrain, Egypt, Iran, Iraq, Israel, Brazil, Bolivia, Chile, Colombia, Costa Rica, Cuba, Dominican Rep., Ecuador, El Salvador, Guinea, Guatemala, Honduras, Martinique, Mexico, Nicaragua, Panama, Paraguay, Peru, Puerto Rico, Uruguay, Venezuela, Albania, Armenia, Azerbaijan, Belarus, Georgia, Kazakhstan, Kosovo, Kyrgyzstan, Macedonia, Moldova, Montenegro, Russia, Serbia, Tajikistan, Turkmenistan, Ukraine, Uzbekistan, Argentina</t>
-  </si>
-  <si>
-    <t>Entrepreneurship School (Social Entrepreneurship)</t>
-  </si>
-  <si>
-    <t>online</t>
-  </si>
-  <si>
-    <t>Enviu</t>
-  </si>
-  <si>
-    <t>Netherlands, Nairobi, Kenya, India, USA</t>
-  </si>
-  <si>
-    <t>Euforia</t>
-  </si>
-  <si>
-    <t>Switzerland, Rwanda, Egypt, Greece, Turkey, Austria, Netherlands, P. of Liechtenstein, France, Germany, Portugal, Colombia, Peru, Bolivia</t>
-  </si>
-  <si>
-    <t>European Social Innovation Competition</t>
-  </si>
-  <si>
-    <t>Iceland, Norway, Albania, Bosnia and Herz., Macedonia, Montenegro, Serbia, Turkey, Israel, Moldova, Switzerland, Faroe Islands, Ukraine, Tunisia, Georgia, Armenia</t>
-  </si>
-  <si>
-    <t>EY - Entrepreneur of the Year</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Canada, Indonesia, Philippines </t>
-  </si>
-  <si>
-    <t>Facebook Social Entrepreneurship Award</t>
-  </si>
-  <si>
-    <t>Fledge</t>
-  </si>
-  <si>
-    <t>Peru, Spain, Italy, Canada, USA</t>
-  </si>
-  <si>
-    <t>Fossil Foundation</t>
-  </si>
-  <si>
-    <t>Canada, USA, Ecuador, Zambia, Kenya, Nigeria, Italy, Switzerland, UK, Poland, India, Cambodia, Laos, China, Hong Kong, Taiwan</t>
-  </si>
-  <si>
-    <t>Global Social Entrepreneurship Network</t>
-  </si>
-  <si>
-    <t>Canada, USA, Europe, Chile, South Africa, Tanzania, Congo, Chad, Morocco, Israel, Cyprus, China, Dem. Rep. Korea, Thailand, Malaysia, Indonesia, Australia, New Zealand, Taiwan</t>
-  </si>
-  <si>
-    <t>Costs</t>
-  </si>
-  <si>
-    <t>Online Courses (1= nur online, 2= beides)</t>
-  </si>
-  <si>
-    <t>Europe</t>
-  </si>
-  <si>
-    <t>Global Social Venture Competition</t>
-  </si>
-  <si>
-    <t>Global Center for Social Entrepreneurship Networks (GCSEN)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Halcyon </t>
-  </si>
-  <si>
-    <t>USA, Saudi Arabia, Dem. Rep. Korea</t>
-  </si>
-  <si>
-    <t>HKCSS Impact Incubator</t>
-  </si>
-  <si>
-    <t>Hult Prize</t>
-  </si>
-  <si>
-    <t>Impact Engine</t>
-  </si>
-  <si>
-    <t>Canada, USA</t>
-  </si>
-  <si>
-    <t>Makesense</t>
-  </si>
-  <si>
-    <t>USA, Canada, Mexico, Dominican Rep., Nicaragua, Guatemala, Trinidad and Tobago, Colombia, Argentina, Paraguay, Brazil, Europe, Morocco, Tunisia, South Africa, Australia, Lebanon, Mali, Burkina Faso, Cote d'Ivoire, Senegal, Togo, Uganda, Kenya, Egypt, Turkey, Armenia, Teheran, Nepal, India, China, Myanmar, Cambodia, Vietnam, Malaysia, Singapore, Indonesia, Philippines, Dem. Rep. Korea, Japan, New Zealand</t>
-  </si>
-  <si>
-    <t>MassChallenge</t>
-  </si>
-  <si>
-    <t>USA, Israel, Mexico, Switzerland, UK</t>
-  </si>
-  <si>
-    <t>Middlesex University London (Social Enterprise: Turning Ideas into Action)</t>
-  </si>
-  <si>
-    <t>Miller Center for Social Entrepreneurship - Global Social Benefit Institute</t>
-  </si>
-  <si>
-    <t>Ogunte</t>
-  </si>
-  <si>
-    <t>Orange Social Venture Prize</t>
-  </si>
-  <si>
-    <t>Morocco, Tunisia, Egypt, Senegal, Botswana, Liberia, cote d'ivoire, Cameroon, Mali, Guinea , Guinea-Bissau, Madagascar, Niger, Central African Rep., Dem. Rep. Congo, Jordan, Burkina Faso</t>
-  </si>
-  <si>
-    <t>Acumen</t>
-  </si>
-  <si>
-    <t>Schwab Foundation for Social Entrepreneurship</t>
-  </si>
-  <si>
-    <t>Seakademie</t>
-  </si>
-  <si>
-    <t>Mexico, South Africa, China, Germany</t>
-  </si>
-  <si>
-    <t>SEED Initiative</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Colombia, India, Tanzania, Thailand, Uganda </t>
-  </si>
-  <si>
-    <t>Seedstars</t>
   </si>
   <si>
     <t>Segal Family Foundation</t>
@@ -2289,12 +2292,12 @@
         <v>1.0</v>
       </c>
       <c r="O39" s="6" t="s">
-        <v>34</v>
+        <v>79</v>
       </c>
     </row>
     <row r="40" ht="19.5" customHeight="1">
       <c r="A40" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B40" s="4">
         <v>1.0</v>
@@ -2336,12 +2339,12 @@
         <v>0.0</v>
       </c>
       <c r="O40" s="4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="41" ht="19.5" customHeight="1">
       <c r="A41" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B41" s="4">
         <v>0.0</v>
@@ -2388,7 +2391,7 @@
     </row>
     <row r="42" ht="19.5" customHeight="1">
       <c r="A42" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B42" s="4">
         <v>0.0</v>
@@ -2435,7 +2438,7 @@
     </row>
     <row r="43" ht="19.5" customHeight="1">
       <c r="A43" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B43" s="4">
         <v>0.0</v>
@@ -2477,12 +2480,12 @@
         <v>0.0</v>
       </c>
       <c r="O43" s="4" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="44" ht="19.5" customHeight="1">
       <c r="A44" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B44" s="4">
         <v>0.0</v>
@@ -2573,7 +2576,7 @@
     </row>
     <row r="46" ht="19.5" customHeight="1">
       <c r="A46" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B46" s="4">
         <v>0.0</v>
@@ -2615,12 +2618,12 @@
         <v>1.0</v>
       </c>
       <c r="O46" s="4" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="47" ht="19.5" customHeight="1">
       <c r="A47" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B47" s="4">
         <v>0.0</v>
@@ -2662,12 +2665,12 @@
         <v>0.0</v>
       </c>
       <c r="O47" s="4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="48" ht="19.5" customHeight="1">
       <c r="A48" s="4" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B48" s="4">
         <v>0.0</v>
@@ -2714,7 +2717,7 @@
     </row>
     <row r="49" ht="19.5" customHeight="1">
       <c r="A49" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B49" s="4">
         <v>0.0</v>
@@ -2761,7 +2764,7 @@
     </row>
     <row r="50" ht="19.5" customHeight="1">
       <c r="A50" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B50" s="4">
         <v>1.0</v>
@@ -2803,12 +2806,12 @@
         <v>1.0</v>
       </c>
       <c r="O50" s="5" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="51" ht="19.5" customHeight="1">
       <c r="A51" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B51" s="4">
         <v>0.0</v>
@@ -2850,12 +2853,12 @@
         <v>0.0</v>
       </c>
       <c r="O51" s="4" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="52" ht="19.5" customHeight="1">
       <c r="A52" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B52" s="4">
         <v>0.0</v>
@@ -2897,12 +2900,12 @@
         <v>0.0</v>
       </c>
       <c r="O52" s="4" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="53" ht="19.5" customHeight="1">
       <c r="A53" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B53" s="4">
         <v>1.0</v>
@@ -2949,7 +2952,7 @@
     </row>
     <row r="54" ht="19.5" customHeight="1">
       <c r="A54" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B54" s="4">
         <v>1.0</v>
@@ -2969,7 +2972,7 @@
     </row>
     <row r="55" ht="19.5" customHeight="1">
       <c r="A55" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B55" s="4">
         <v>1.0</v>
@@ -3011,12 +3014,12 @@
         <v>0.0</v>
       </c>
       <c r="O55" s="5" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="56" ht="19.5" customHeight="1">
       <c r="A56" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B56" s="4">
         <v>1.0</v>
@@ -3063,7 +3066,7 @@
     </row>
     <row r="57" ht="19.5" customHeight="1">
       <c r="A57" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B57" s="4">
         <v>1.0</v>
@@ -3110,7 +3113,7 @@
     </row>
     <row r="58" ht="19.5" customHeight="1">
       <c r="A58" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B58" s="4">
         <v>1.0</v>
@@ -3152,12 +3155,12 @@
         <v>0.0</v>
       </c>
       <c r="O58" s="4" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="59" ht="19.5" customHeight="1">
       <c r="A59" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B59" s="4">
         <v>1.0</v>
@@ -3204,7 +3207,7 @@
     </row>
     <row r="60" ht="19.5" customHeight="1">
       <c r="A60" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B60" s="4">
         <v>0.0</v>
@@ -3246,12 +3249,12 @@
         <v>0.0</v>
       </c>
       <c r="O60" s="4" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="61" ht="19.5" customHeight="1">
       <c r="A61" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B61" s="4">
         <v>1.0</v>
@@ -3293,7 +3296,7 @@
         <v>0.0</v>
       </c>
       <c r="O61" s="5" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="62" ht="15.75" customHeight="1">
@@ -3328,7 +3331,7 @@
         <v>9</v>
       </c>
       <c r="K62" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="L62" s="1" t="s">
         <v>11</v>
@@ -3342,7 +3345,7 @@
     </row>
     <row r="63" ht="15.75" customHeight="1">
       <c r="A63" s="4" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B63" s="4">
         <v>1.0</v>
@@ -3384,7 +3387,7 @@
         <v>0.0</v>
       </c>
       <c r="O63" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="64" ht="15.75" customHeight="1"/>

</xml_diff>